<commit_message>
pasted initial requirements for traceability
</commit_message>
<xml_diff>
--- a/OntoGSN Competency Questions.xlsx
+++ b/OntoGSN Competency Questions.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\momcilovic\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\momcilovic\Documents\GitHub\OntoGSN_fortiss\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DB80A83-D6B0-4D71-B114-A6897CEFFED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86FBAFB8-2879-425A-823F-BC62D5D90582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{2AA26972-218B-47B4-A46D-EEBC3B18A819}"/>
+    <workbookView xWindow="55428" yWindow="2268" windowWidth="23040" windowHeight="12204" activeTab="1" xr2:uid="{2AA26972-218B-47B4-A46D-EEBC3B18A819}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Competency Questions" sheetId="1" r:id="rId1"/>
+    <sheet name="Initial Requirements" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="75">
   <si>
     <t>Assurance engineer</t>
   </si>
@@ -189,6 +190,78 @@
   </si>
   <si>
     <t>find_solutions_with_confidence.rq</t>
+  </si>
+  <si>
+    <t>Requirement</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>User should be capable of performing every aspect in the normative GSN v3 standard with OntoGSN.</t>
+  </si>
+  <si>
+    <t>OntoGSN should represent knowledge about GSN assurance cases in direct conformity with the standard metamodel.</t>
+  </si>
+  <si>
+    <t>OntoGSN should be aligned with the ASCE XML schema.</t>
+  </si>
+  <si>
+    <t>The user should be able to use OntoGSN as a standalone framework.</t>
+  </si>
+  <si>
+    <t>The user should be able to use OntoGSN in an accessible manner.</t>
+  </si>
+  <si>
+    <t>OntoGSN should not duplicate the features provided by existing tools and frameworks (e.g., GUI, imports/exports).</t>
+  </si>
+  <si>
+    <t>The user should have an accessible and easy way to create SPARQL queries based on a case ABox conformant to the OntoGSN TBox.</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>refers to</t>
+  </si>
+  <si>
+    <t>ontology</t>
+  </si>
+  <si>
+    <t>framework, supporting tools</t>
+  </si>
+  <si>
+    <t>supporting tools</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>GSN Standard</t>
+  </si>
+  <si>
+    <t>https://scsc.uk/index.php/tools</t>
+  </si>
+  <si>
+    <t>https://scsc.uk/index.php/tools; feedback</t>
+  </si>
+  <si>
+    <t>feedback</t>
   </si>
 </sst>
 </file>
@@ -238,7 +311,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -247,6 +320,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -583,8 +657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6658B5FA-63AD-4D48-9689-BAC92E93E4EF}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -822,4 +896,130 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D979CF69-1B15-45B8-A085-107B992ECEFC}">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="38.88671875" customWidth="1"/>
+    <col min="3" max="3" width="25.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>